<commit_message>
New manual growth data
</commit_message>
<xml_diff>
--- a/data/sizes/B_2023POGS_small_seed_daily/B_sizes_06252025.xlsx
+++ b/data/sizes/B_2023POGS_small_seed_daily/B_sizes_06252025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceleuchtenberger/Library/Mobile Documents/com~apple~CloudDocs/Documents/project-gigas-conditioning-GL/data/sizes/B_2023POGS_small_seed_daily/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20D14B9D-06D0-DF4E-9ABD-74D008907317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E6D1D7-E537-BF47-9DC2-9F98D2D4DD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8100" yWindow="1280" windowWidth="24840" windowHeight="17160" xr2:uid="{59562AC7-2699-D84F-A30D-CDAA438C0A0D}"/>
+    <workbookView xWindow="5760" yWindow="940" windowWidth="24840" windowHeight="17160" xr2:uid="{59562AC7-2699-D84F-A30D-CDAA438C0A0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6156" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6522" uniqueCount="35">
   <si>
     <t>effort</t>
   </si>
@@ -514,11 +514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{951AA300-CB28-DA47-A4F6-6DBA5477955B}">
-  <dimension ref="A1:XFD911"/>
+  <dimension ref="A1:XFD981"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A893" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I907" sqref="I907"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="163" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A955" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L976" sqref="L976"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -44710,6 +44710,2735 @@
         <v>#N/A</v>
       </c>
     </row>
+    <row r="912" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A912" t="s">
+        <v>11</v>
+      </c>
+      <c r="B912" t="s">
+        <v>12</v>
+      </c>
+      <c r="C912" t="s">
+        <v>13</v>
+      </c>
+      <c r="D912" t="s">
+        <v>14</v>
+      </c>
+      <c r="E912" t="s">
+        <v>15</v>
+      </c>
+      <c r="F912" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G912" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H912">
+        <v>7</v>
+      </c>
+      <c r="I912">
+        <v>77</v>
+      </c>
+      <c r="J912" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K912">
+        <v>77.09</v>
+      </c>
+      <c r="L912">
+        <v>50.83</v>
+      </c>
+      <c r="M912">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="N912" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="913" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A913" t="s">
+        <v>11</v>
+      </c>
+      <c r="B913" t="s">
+        <v>12</v>
+      </c>
+      <c r="C913" t="s">
+        <v>13</v>
+      </c>
+      <c r="D913" t="s">
+        <v>14</v>
+      </c>
+      <c r="E913" t="s">
+        <v>15</v>
+      </c>
+      <c r="F913" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G913" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H913">
+        <v>7</v>
+      </c>
+      <c r="I913">
+        <v>77</v>
+      </c>
+      <c r="J913" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K913">
+        <v>46.51</v>
+      </c>
+      <c r="L913">
+        <v>33.25</v>
+      </c>
+      <c r="M913">
+        <v>16.010000000000002</v>
+      </c>
+      <c r="N913" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="914" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A914" t="s">
+        <v>11</v>
+      </c>
+      <c r="B914" t="s">
+        <v>12</v>
+      </c>
+      <c r="C914" t="s">
+        <v>13</v>
+      </c>
+      <c r="D914" t="s">
+        <v>14</v>
+      </c>
+      <c r="E914" t="s">
+        <v>15</v>
+      </c>
+      <c r="F914" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G914" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H914">
+        <v>7</v>
+      </c>
+      <c r="I914">
+        <v>77</v>
+      </c>
+      <c r="J914" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K914">
+        <v>69.14</v>
+      </c>
+      <c r="L914">
+        <v>47.74</v>
+      </c>
+      <c r="M914">
+        <v>20.6</v>
+      </c>
+      <c r="N914" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="915" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A915" t="s">
+        <v>11</v>
+      </c>
+      <c r="B915" t="s">
+        <v>12</v>
+      </c>
+      <c r="C915" t="s">
+        <v>13</v>
+      </c>
+      <c r="D915" t="s">
+        <v>14</v>
+      </c>
+      <c r="E915" t="s">
+        <v>15</v>
+      </c>
+      <c r="F915" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G915" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H915">
+        <v>7</v>
+      </c>
+      <c r="I915">
+        <v>77</v>
+      </c>
+      <c r="J915" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K915">
+        <v>51.08</v>
+      </c>
+      <c r="L915">
+        <v>28.55</v>
+      </c>
+      <c r="M915">
+        <v>15.2</v>
+      </c>
+      <c r="N915" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="916" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A916" t="s">
+        <v>11</v>
+      </c>
+      <c r="B916" t="s">
+        <v>12</v>
+      </c>
+      <c r="C916" t="s">
+        <v>13</v>
+      </c>
+      <c r="D916" t="s">
+        <v>14</v>
+      </c>
+      <c r="E916" t="s">
+        <v>15</v>
+      </c>
+      <c r="F916" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G916" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H916">
+        <v>7</v>
+      </c>
+      <c r="I916">
+        <v>77</v>
+      </c>
+      <c r="J916" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K916">
+        <v>64.22</v>
+      </c>
+      <c r="L916">
+        <v>50.58</v>
+      </c>
+      <c r="M916">
+        <v>16.48</v>
+      </c>
+      <c r="N916" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="917" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A917" t="s">
+        <v>11</v>
+      </c>
+      <c r="B917" t="s">
+        <v>12</v>
+      </c>
+      <c r="C917" t="s">
+        <v>13</v>
+      </c>
+      <c r="D917" t="s">
+        <v>14</v>
+      </c>
+      <c r="E917" t="s">
+        <v>15</v>
+      </c>
+      <c r="F917" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G917" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H917">
+        <v>7</v>
+      </c>
+      <c r="I917">
+        <v>77</v>
+      </c>
+      <c r="J917" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K917">
+        <v>82.69</v>
+      </c>
+      <c r="L917">
+        <v>41.9</v>
+      </c>
+      <c r="M917">
+        <v>17.78</v>
+      </c>
+      <c r="N917" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="918" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A918" t="s">
+        <v>11</v>
+      </c>
+      <c r="B918" t="s">
+        <v>12</v>
+      </c>
+      <c r="C918" t="s">
+        <v>13</v>
+      </c>
+      <c r="D918" t="s">
+        <v>14</v>
+      </c>
+      <c r="E918" t="s">
+        <v>15</v>
+      </c>
+      <c r="F918" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G918" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H918">
+        <v>7</v>
+      </c>
+      <c r="I918">
+        <v>77</v>
+      </c>
+      <c r="J918" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K918">
+        <v>50.5</v>
+      </c>
+      <c r="L918">
+        <v>38.159999999999997</v>
+      </c>
+      <c r="M918">
+        <v>20.93</v>
+      </c>
+      <c r="N918" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="919" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A919" t="s">
+        <v>11</v>
+      </c>
+      <c r="B919" t="s">
+        <v>12</v>
+      </c>
+      <c r="C919" t="s">
+        <v>13</v>
+      </c>
+      <c r="D919" t="s">
+        <v>14</v>
+      </c>
+      <c r="E919" t="s">
+        <v>15</v>
+      </c>
+      <c r="F919" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G919" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H919">
+        <v>7</v>
+      </c>
+      <c r="I919">
+        <v>77</v>
+      </c>
+      <c r="J919" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K919">
+        <v>57.81</v>
+      </c>
+      <c r="L919">
+        <v>49.53</v>
+      </c>
+      <c r="M919">
+        <v>19.75</v>
+      </c>
+      <c r="N919" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="920" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A920" t="s">
+        <v>11</v>
+      </c>
+      <c r="B920" t="s">
+        <v>12</v>
+      </c>
+      <c r="C920" t="s">
+        <v>13</v>
+      </c>
+      <c r="D920" t="s">
+        <v>14</v>
+      </c>
+      <c r="E920" t="s">
+        <v>15</v>
+      </c>
+      <c r="F920" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G920" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H920">
+        <v>7</v>
+      </c>
+      <c r="I920">
+        <v>77</v>
+      </c>
+      <c r="J920" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K920">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="L920">
+        <v>41.27</v>
+      </c>
+      <c r="M920">
+        <v>15.91</v>
+      </c>
+      <c r="N920" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="921" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A921" t="s">
+        <v>11</v>
+      </c>
+      <c r="B921" t="s">
+        <v>12</v>
+      </c>
+      <c r="C921" t="s">
+        <v>13</v>
+      </c>
+      <c r="D921" t="s">
+        <v>14</v>
+      </c>
+      <c r="E921" t="s">
+        <v>15</v>
+      </c>
+      <c r="F921" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G921" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H921">
+        <v>7</v>
+      </c>
+      <c r="I921">
+        <v>77</v>
+      </c>
+      <c r="J921" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K921">
+        <v>48.28</v>
+      </c>
+      <c r="L921">
+        <v>39.520000000000003</v>
+      </c>
+      <c r="M921">
+        <v>13.57</v>
+      </c>
+      <c r="N921" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="922" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A922" t="s">
+        <v>11</v>
+      </c>
+      <c r="B922" t="s">
+        <v>12</v>
+      </c>
+      <c r="C922" t="s">
+        <v>13</v>
+      </c>
+      <c r="D922" t="s">
+        <v>16</v>
+      </c>
+      <c r="E922" t="s">
+        <v>15</v>
+      </c>
+      <c r="F922" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G922" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H922">
+        <v>2</v>
+      </c>
+      <c r="I922">
+        <v>78</v>
+      </c>
+      <c r="J922" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K922">
+        <v>76.58</v>
+      </c>
+      <c r="L922">
+        <v>38.46</v>
+      </c>
+      <c r="M922">
+        <v>17.12</v>
+      </c>
+      <c r="N922" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="923" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A923" t="s">
+        <v>11</v>
+      </c>
+      <c r="B923" t="s">
+        <v>12</v>
+      </c>
+      <c r="C923" t="s">
+        <v>13</v>
+      </c>
+      <c r="D923" t="s">
+        <v>16</v>
+      </c>
+      <c r="E923" t="s">
+        <v>15</v>
+      </c>
+      <c r="F923" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G923" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H923">
+        <v>2</v>
+      </c>
+      <c r="I923">
+        <v>78</v>
+      </c>
+      <c r="J923" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K923">
+        <v>44.79</v>
+      </c>
+      <c r="L923">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="M923">
+        <v>11.07</v>
+      </c>
+      <c r="N923" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="924" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A924" t="s">
+        <v>11</v>
+      </c>
+      <c r="B924" t="s">
+        <v>12</v>
+      </c>
+      <c r="C924" t="s">
+        <v>13</v>
+      </c>
+      <c r="D924" t="s">
+        <v>16</v>
+      </c>
+      <c r="E924" t="s">
+        <v>15</v>
+      </c>
+      <c r="F924" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G924" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H924">
+        <v>2</v>
+      </c>
+      <c r="I924">
+        <v>78</v>
+      </c>
+      <c r="J924" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K924">
+        <v>52.96</v>
+      </c>
+      <c r="L924">
+        <v>40.26</v>
+      </c>
+      <c r="M924">
+        <v>24.64</v>
+      </c>
+      <c r="N924" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="925" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A925" t="s">
+        <v>11</v>
+      </c>
+      <c r="B925" t="s">
+        <v>12</v>
+      </c>
+      <c r="C925" t="s">
+        <v>13</v>
+      </c>
+      <c r="D925" t="s">
+        <v>16</v>
+      </c>
+      <c r="E925" t="s">
+        <v>15</v>
+      </c>
+      <c r="F925" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G925" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H925">
+        <v>2</v>
+      </c>
+      <c r="I925">
+        <v>78</v>
+      </c>
+      <c r="J925" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K925">
+        <v>71.84</v>
+      </c>
+      <c r="L925">
+        <v>36.979999999999997</v>
+      </c>
+      <c r="M925">
+        <v>17.510000000000002</v>
+      </c>
+      <c r="N925" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="926" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A926" t="s">
+        <v>11</v>
+      </c>
+      <c r="B926" t="s">
+        <v>12</v>
+      </c>
+      <c r="C926" t="s">
+        <v>13</v>
+      </c>
+      <c r="D926" t="s">
+        <v>16</v>
+      </c>
+      <c r="E926" t="s">
+        <v>15</v>
+      </c>
+      <c r="F926" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G926" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H926">
+        <v>2</v>
+      </c>
+      <c r="I926">
+        <v>78</v>
+      </c>
+      <c r="J926" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K926">
+        <v>66.2</v>
+      </c>
+      <c r="L926">
+        <v>48.4</v>
+      </c>
+      <c r="M926">
+        <v>20.27</v>
+      </c>
+      <c r="N926" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="927" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A927" t="s">
+        <v>11</v>
+      </c>
+      <c r="B927" t="s">
+        <v>12</v>
+      </c>
+      <c r="C927" t="s">
+        <v>13</v>
+      </c>
+      <c r="D927" t="s">
+        <v>16</v>
+      </c>
+      <c r="E927" t="s">
+        <v>15</v>
+      </c>
+      <c r="F927" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G927" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H927">
+        <v>2</v>
+      </c>
+      <c r="I927">
+        <v>78</v>
+      </c>
+      <c r="J927" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K927">
+        <v>51.1</v>
+      </c>
+      <c r="L927">
+        <v>37.909999999999997</v>
+      </c>
+      <c r="M927">
+        <v>20.86</v>
+      </c>
+      <c r="N927" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="928" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A928" t="s">
+        <v>11</v>
+      </c>
+      <c r="B928" t="s">
+        <v>12</v>
+      </c>
+      <c r="C928" t="s">
+        <v>13</v>
+      </c>
+      <c r="D928" t="s">
+        <v>16</v>
+      </c>
+      <c r="E928" t="s">
+        <v>15</v>
+      </c>
+      <c r="F928" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G928" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H928">
+        <v>2</v>
+      </c>
+      <c r="I928">
+        <v>78</v>
+      </c>
+      <c r="J928" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K928">
+        <v>52.05</v>
+      </c>
+      <c r="L928">
+        <v>37.369999999999997</v>
+      </c>
+      <c r="M928">
+        <v>23.05</v>
+      </c>
+      <c r="N928" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="929" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A929" t="s">
+        <v>11</v>
+      </c>
+      <c r="B929" t="s">
+        <v>12</v>
+      </c>
+      <c r="C929" t="s">
+        <v>13</v>
+      </c>
+      <c r="D929" t="s">
+        <v>16</v>
+      </c>
+      <c r="E929" t="s">
+        <v>15</v>
+      </c>
+      <c r="F929" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G929" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H929">
+        <v>2</v>
+      </c>
+      <c r="I929">
+        <v>78</v>
+      </c>
+      <c r="J929" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K929">
+        <v>53.23</v>
+      </c>
+      <c r="L929">
+        <v>34.57</v>
+      </c>
+      <c r="M929">
+        <v>15.36</v>
+      </c>
+      <c r="N929" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="930" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A930" t="s">
+        <v>11</v>
+      </c>
+      <c r="B930" t="s">
+        <v>12</v>
+      </c>
+      <c r="C930" t="s">
+        <v>13</v>
+      </c>
+      <c r="D930" t="s">
+        <v>16</v>
+      </c>
+      <c r="E930" t="s">
+        <v>15</v>
+      </c>
+      <c r="F930" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G930" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H930">
+        <v>2</v>
+      </c>
+      <c r="I930">
+        <v>78</v>
+      </c>
+      <c r="J930" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K930">
+        <v>71.03</v>
+      </c>
+      <c r="L930">
+        <v>40.29</v>
+      </c>
+      <c r="M930">
+        <v>14.29</v>
+      </c>
+      <c r="N930" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="931" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A931" t="s">
+        <v>11</v>
+      </c>
+      <c r="B931" t="s">
+        <v>12</v>
+      </c>
+      <c r="C931" t="s">
+        <v>13</v>
+      </c>
+      <c r="D931" t="s">
+        <v>16</v>
+      </c>
+      <c r="E931" t="s">
+        <v>15</v>
+      </c>
+      <c r="F931" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G931" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H931">
+        <v>2</v>
+      </c>
+      <c r="I931">
+        <v>78</v>
+      </c>
+      <c r="J931" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K931">
+        <v>48.47</v>
+      </c>
+      <c r="L931">
+        <v>31.32</v>
+      </c>
+      <c r="M931">
+        <v>14.44</v>
+      </c>
+      <c r="N931" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="932" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A932" t="s">
+        <v>11</v>
+      </c>
+      <c r="B932" t="s">
+        <v>12</v>
+      </c>
+      <c r="C932" t="s">
+        <v>13</v>
+      </c>
+      <c r="D932" t="s">
+        <v>16</v>
+      </c>
+      <c r="E932" t="s">
+        <v>15</v>
+      </c>
+      <c r="F932" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G932" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H932">
+        <v>1</v>
+      </c>
+      <c r="I932">
+        <v>53</v>
+      </c>
+      <c r="J932" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K932">
+        <v>72.430000000000007</v>
+      </c>
+      <c r="L932">
+        <v>53.14</v>
+      </c>
+      <c r="M932">
+        <v>18.09</v>
+      </c>
+      <c r="N932" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="933" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A933" t="s">
+        <v>11</v>
+      </c>
+      <c r="B933" t="s">
+        <v>12</v>
+      </c>
+      <c r="C933" t="s">
+        <v>13</v>
+      </c>
+      <c r="D933" t="s">
+        <v>16</v>
+      </c>
+      <c r="E933" t="s">
+        <v>15</v>
+      </c>
+      <c r="F933" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G933" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H933">
+        <v>1</v>
+      </c>
+      <c r="I933">
+        <v>53</v>
+      </c>
+      <c r="J933" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K933">
+        <v>60.57</v>
+      </c>
+      <c r="L933">
+        <v>44.95</v>
+      </c>
+      <c r="M933">
+        <v>21.92</v>
+      </c>
+      <c r="N933" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="934" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A934" t="s">
+        <v>11</v>
+      </c>
+      <c r="B934" t="s">
+        <v>12</v>
+      </c>
+      <c r="C934" t="s">
+        <v>13</v>
+      </c>
+      <c r="D934" t="s">
+        <v>16</v>
+      </c>
+      <c r="E934" t="s">
+        <v>15</v>
+      </c>
+      <c r="F934" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G934" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H934">
+        <v>1</v>
+      </c>
+      <c r="I934">
+        <v>53</v>
+      </c>
+      <c r="J934" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K934">
+        <v>46.8</v>
+      </c>
+      <c r="L934">
+        <v>42.64</v>
+      </c>
+      <c r="M934">
+        <v>14.01</v>
+      </c>
+      <c r="N934" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="935" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A935" t="s">
+        <v>11</v>
+      </c>
+      <c r="B935" t="s">
+        <v>12</v>
+      </c>
+      <c r="C935" t="s">
+        <v>13</v>
+      </c>
+      <c r="D935" t="s">
+        <v>16</v>
+      </c>
+      <c r="E935" t="s">
+        <v>15</v>
+      </c>
+      <c r="F935" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G935" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H935">
+        <v>1</v>
+      </c>
+      <c r="I935">
+        <v>53</v>
+      </c>
+      <c r="J935" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K935">
+        <v>62.36</v>
+      </c>
+      <c r="L935">
+        <v>46.81</v>
+      </c>
+      <c r="M935">
+        <v>15.29</v>
+      </c>
+      <c r="N935" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="936" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A936" t="s">
+        <v>11</v>
+      </c>
+      <c r="B936" t="s">
+        <v>12</v>
+      </c>
+      <c r="C936" t="s">
+        <v>13</v>
+      </c>
+      <c r="D936" t="s">
+        <v>16</v>
+      </c>
+      <c r="E936" t="s">
+        <v>15</v>
+      </c>
+      <c r="F936" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G936" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H936">
+        <v>1</v>
+      </c>
+      <c r="I936">
+        <v>53</v>
+      </c>
+      <c r="J936" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K936">
+        <v>41.89</v>
+      </c>
+      <c r="L936">
+        <v>37.64</v>
+      </c>
+      <c r="M936">
+        <v>12.26</v>
+      </c>
+      <c r="N936" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="937" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A937" t="s">
+        <v>11</v>
+      </c>
+      <c r="B937" t="s">
+        <v>12</v>
+      </c>
+      <c r="C937" t="s">
+        <v>13</v>
+      </c>
+      <c r="D937" t="s">
+        <v>16</v>
+      </c>
+      <c r="E937" t="s">
+        <v>15</v>
+      </c>
+      <c r="F937" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G937" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H937">
+        <v>1</v>
+      </c>
+      <c r="I937">
+        <v>53</v>
+      </c>
+      <c r="J937" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K937">
+        <v>64.25</v>
+      </c>
+      <c r="L937">
+        <v>41.86</v>
+      </c>
+      <c r="M937">
+        <v>24.75</v>
+      </c>
+      <c r="N937" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="938" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A938" t="s">
+        <v>11</v>
+      </c>
+      <c r="B938" t="s">
+        <v>12</v>
+      </c>
+      <c r="C938" t="s">
+        <v>13</v>
+      </c>
+      <c r="D938" t="s">
+        <v>16</v>
+      </c>
+      <c r="E938" t="s">
+        <v>15</v>
+      </c>
+      <c r="F938" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G938" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H938">
+        <v>1</v>
+      </c>
+      <c r="I938">
+        <v>53</v>
+      </c>
+      <c r="J938" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K938">
+        <v>52.36</v>
+      </c>
+      <c r="L938">
+        <v>33.71</v>
+      </c>
+      <c r="M938">
+        <v>22.83</v>
+      </c>
+      <c r="N938" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="939" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A939" t="s">
+        <v>11</v>
+      </c>
+      <c r="B939" t="s">
+        <v>12</v>
+      </c>
+      <c r="C939" t="s">
+        <v>13</v>
+      </c>
+      <c r="D939" t="s">
+        <v>16</v>
+      </c>
+      <c r="E939" t="s">
+        <v>15</v>
+      </c>
+      <c r="F939" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G939" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H939">
+        <v>1</v>
+      </c>
+      <c r="I939">
+        <v>53</v>
+      </c>
+      <c r="J939" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K939">
+        <v>68.150000000000006</v>
+      </c>
+      <c r="L939">
+        <v>32.94</v>
+      </c>
+      <c r="M939">
+        <v>16.36</v>
+      </c>
+      <c r="N939" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="940" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A940" t="s">
+        <v>11</v>
+      </c>
+      <c r="B940" t="s">
+        <v>12</v>
+      </c>
+      <c r="C940" t="s">
+        <v>13</v>
+      </c>
+      <c r="D940" t="s">
+        <v>16</v>
+      </c>
+      <c r="E940" t="s">
+        <v>15</v>
+      </c>
+      <c r="F940" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G940" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H940">
+        <v>1</v>
+      </c>
+      <c r="I940">
+        <v>53</v>
+      </c>
+      <c r="J940" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K940">
+        <v>54.27</v>
+      </c>
+      <c r="L940">
+        <v>52.65</v>
+      </c>
+      <c r="M940">
+        <v>17.63</v>
+      </c>
+      <c r="N940" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="941" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A941" t="s">
+        <v>11</v>
+      </c>
+      <c r="B941" t="s">
+        <v>12</v>
+      </c>
+      <c r="C941" t="s">
+        <v>13</v>
+      </c>
+      <c r="D941" t="s">
+        <v>16</v>
+      </c>
+      <c r="E941" t="s">
+        <v>15</v>
+      </c>
+      <c r="F941" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G941" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H941">
+        <v>1</v>
+      </c>
+      <c r="I941">
+        <v>53</v>
+      </c>
+      <c r="J941" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K941">
+        <v>51.91</v>
+      </c>
+      <c r="L941">
+        <v>41.34</v>
+      </c>
+      <c r="M941">
+        <v>18.28</v>
+      </c>
+      <c r="N941" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="942" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A942" t="s">
+        <v>11</v>
+      </c>
+      <c r="B942" t="s">
+        <v>12</v>
+      </c>
+      <c r="C942" t="s">
+        <v>13</v>
+      </c>
+      <c r="D942" t="s">
+        <v>14</v>
+      </c>
+      <c r="E942" t="s">
+        <v>15</v>
+      </c>
+      <c r="F942" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G942" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H942">
+        <v>6</v>
+      </c>
+      <c r="I942">
+        <v>67</v>
+      </c>
+      <c r="J942" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K942">
+        <v>70.86</v>
+      </c>
+      <c r="L942">
+        <v>34.549999999999997</v>
+      </c>
+      <c r="M942">
+        <v>15.08</v>
+      </c>
+      <c r="N942" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="943" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A943" t="s">
+        <v>11</v>
+      </c>
+      <c r="B943" t="s">
+        <v>12</v>
+      </c>
+      <c r="C943" t="s">
+        <v>13</v>
+      </c>
+      <c r="D943" t="s">
+        <v>14</v>
+      </c>
+      <c r="E943" t="s">
+        <v>15</v>
+      </c>
+      <c r="F943" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G943" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H943">
+        <v>6</v>
+      </c>
+      <c r="I943">
+        <v>67</v>
+      </c>
+      <c r="J943" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K943">
+        <v>41.69</v>
+      </c>
+      <c r="L943">
+        <v>27.87</v>
+      </c>
+      <c r="M943">
+        <v>13</v>
+      </c>
+      <c r="N943" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="944" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A944" t="s">
+        <v>11</v>
+      </c>
+      <c r="B944" t="s">
+        <v>12</v>
+      </c>
+      <c r="C944" t="s">
+        <v>13</v>
+      </c>
+      <c r="D944" t="s">
+        <v>14</v>
+      </c>
+      <c r="E944" t="s">
+        <v>15</v>
+      </c>
+      <c r="F944" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G944" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H944">
+        <v>6</v>
+      </c>
+      <c r="I944">
+        <v>67</v>
+      </c>
+      <c r="J944" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K944">
+        <v>49.84</v>
+      </c>
+      <c r="L944">
+        <v>41.08</v>
+      </c>
+      <c r="M944">
+        <v>14.75</v>
+      </c>
+      <c r="N944" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="945" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A945" t="s">
+        <v>11</v>
+      </c>
+      <c r="B945" t="s">
+        <v>12</v>
+      </c>
+      <c r="C945" t="s">
+        <v>13</v>
+      </c>
+      <c r="D945" t="s">
+        <v>14</v>
+      </c>
+      <c r="E945" t="s">
+        <v>15</v>
+      </c>
+      <c r="F945" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G945" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H945">
+        <v>6</v>
+      </c>
+      <c r="I945">
+        <v>67</v>
+      </c>
+      <c r="J945" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K945">
+        <v>67.64</v>
+      </c>
+      <c r="L945">
+        <v>44.04</v>
+      </c>
+      <c r="M945">
+        <v>20.309999999999999</v>
+      </c>
+      <c r="N945" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="946" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A946" t="s">
+        <v>11</v>
+      </c>
+      <c r="B946" t="s">
+        <v>12</v>
+      </c>
+      <c r="C946" t="s">
+        <v>13</v>
+      </c>
+      <c r="D946" t="s">
+        <v>14</v>
+      </c>
+      <c r="E946" t="s">
+        <v>15</v>
+      </c>
+      <c r="F946" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G946" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H946">
+        <v>6</v>
+      </c>
+      <c r="I946">
+        <v>67</v>
+      </c>
+      <c r="J946" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K946">
+        <v>51.54</v>
+      </c>
+      <c r="L946">
+        <v>47.84</v>
+      </c>
+      <c r="M946">
+        <v>21.37</v>
+      </c>
+      <c r="N946" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="947" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A947" t="s">
+        <v>11</v>
+      </c>
+      <c r="B947" t="s">
+        <v>12</v>
+      </c>
+      <c r="C947" t="s">
+        <v>13</v>
+      </c>
+      <c r="D947" t="s">
+        <v>14</v>
+      </c>
+      <c r="E947" t="s">
+        <v>15</v>
+      </c>
+      <c r="F947" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G947" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H947">
+        <v>6</v>
+      </c>
+      <c r="I947">
+        <v>67</v>
+      </c>
+      <c r="J947" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K947">
+        <v>66.72</v>
+      </c>
+      <c r="L947">
+        <v>44.76</v>
+      </c>
+      <c r="M947">
+        <v>19.920000000000002</v>
+      </c>
+      <c r="N947" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="948" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A948" t="s">
+        <v>11</v>
+      </c>
+      <c r="B948" t="s">
+        <v>12</v>
+      </c>
+      <c r="C948" t="s">
+        <v>13</v>
+      </c>
+      <c r="D948" t="s">
+        <v>14</v>
+      </c>
+      <c r="E948" t="s">
+        <v>15</v>
+      </c>
+      <c r="F948" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G948" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H948">
+        <v>6</v>
+      </c>
+      <c r="I948">
+        <v>67</v>
+      </c>
+      <c r="J948" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K948">
+        <v>57.83</v>
+      </c>
+      <c r="L948">
+        <v>42.93</v>
+      </c>
+      <c r="M948">
+        <v>18.670000000000002</v>
+      </c>
+      <c r="N948" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="949" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A949" t="s">
+        <v>11</v>
+      </c>
+      <c r="B949" t="s">
+        <v>12</v>
+      </c>
+      <c r="C949" t="s">
+        <v>13</v>
+      </c>
+      <c r="D949" t="s">
+        <v>14</v>
+      </c>
+      <c r="E949" t="s">
+        <v>15</v>
+      </c>
+      <c r="F949" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G949" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H949">
+        <v>6</v>
+      </c>
+      <c r="I949">
+        <v>67</v>
+      </c>
+      <c r="J949" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K949">
+        <v>67.86</v>
+      </c>
+      <c r="L949">
+        <v>37.31</v>
+      </c>
+      <c r="M949">
+        <v>20.75</v>
+      </c>
+      <c r="N949" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="950" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A950" t="s">
+        <v>11</v>
+      </c>
+      <c r="B950" t="s">
+        <v>12</v>
+      </c>
+      <c r="C950" t="s">
+        <v>13</v>
+      </c>
+      <c r="D950" t="s">
+        <v>14</v>
+      </c>
+      <c r="E950" t="s">
+        <v>15</v>
+      </c>
+      <c r="F950" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G950" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H950">
+        <v>6</v>
+      </c>
+      <c r="I950">
+        <v>67</v>
+      </c>
+      <c r="J950" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K950">
+        <v>63.85</v>
+      </c>
+      <c r="L950">
+        <v>47.76</v>
+      </c>
+      <c r="M950">
+        <v>29.45</v>
+      </c>
+      <c r="N950" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="951" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A951" t="s">
+        <v>11</v>
+      </c>
+      <c r="B951" t="s">
+        <v>12</v>
+      </c>
+      <c r="C951" t="s">
+        <v>13</v>
+      </c>
+      <c r="D951" t="s">
+        <v>14</v>
+      </c>
+      <c r="E951" t="s">
+        <v>15</v>
+      </c>
+      <c r="F951" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G951" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H951">
+        <v>6</v>
+      </c>
+      <c r="I951">
+        <v>67</v>
+      </c>
+      <c r="J951" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K951">
+        <v>45.96</v>
+      </c>
+      <c r="L951">
+        <v>32.64</v>
+      </c>
+      <c r="M951">
+        <v>12.34</v>
+      </c>
+      <c r="N951" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="952" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A952" t="s">
+        <v>11</v>
+      </c>
+      <c r="B952" t="s">
+        <v>12</v>
+      </c>
+      <c r="C952" t="s">
+        <v>13</v>
+      </c>
+      <c r="D952" t="s">
+        <v>16</v>
+      </c>
+      <c r="E952" t="s">
+        <v>15</v>
+      </c>
+      <c r="F952" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G952" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H952">
+        <v>3</v>
+      </c>
+      <c r="I952">
+        <v>59</v>
+      </c>
+      <c r="J952" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K952">
+        <v>60.78</v>
+      </c>
+      <c r="L952">
+        <v>43.09</v>
+      </c>
+      <c r="M952">
+        <v>13.13</v>
+      </c>
+      <c r="N952" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="953" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A953" t="s">
+        <v>11</v>
+      </c>
+      <c r="B953" t="s">
+        <v>12</v>
+      </c>
+      <c r="C953" t="s">
+        <v>13</v>
+      </c>
+      <c r="D953" t="s">
+        <v>16</v>
+      </c>
+      <c r="E953" t="s">
+        <v>15</v>
+      </c>
+      <c r="F953" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G953" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H953">
+        <v>3</v>
+      </c>
+      <c r="I953">
+        <v>59</v>
+      </c>
+      <c r="J953" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K953">
+        <v>88.28</v>
+      </c>
+      <c r="L953">
+        <v>49.11</v>
+      </c>
+      <c r="M953">
+        <v>19.71</v>
+      </c>
+      <c r="N953" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="954" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A954" t="s">
+        <v>11</v>
+      </c>
+      <c r="B954" t="s">
+        <v>12</v>
+      </c>
+      <c r="C954" t="s">
+        <v>13</v>
+      </c>
+      <c r="D954" t="s">
+        <v>16</v>
+      </c>
+      <c r="E954" t="s">
+        <v>15</v>
+      </c>
+      <c r="F954" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G954" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H954">
+        <v>3</v>
+      </c>
+      <c r="I954">
+        <v>59</v>
+      </c>
+      <c r="J954" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K954">
+        <v>44.62</v>
+      </c>
+      <c r="L954">
+        <v>30.22</v>
+      </c>
+      <c r="M954">
+        <v>12.62</v>
+      </c>
+      <c r="N954" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="955" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A955" t="s">
+        <v>11</v>
+      </c>
+      <c r="B955" t="s">
+        <v>12</v>
+      </c>
+      <c r="C955" t="s">
+        <v>13</v>
+      </c>
+      <c r="D955" t="s">
+        <v>16</v>
+      </c>
+      <c r="E955" t="s">
+        <v>15</v>
+      </c>
+      <c r="F955" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G955" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H955">
+        <v>3</v>
+      </c>
+      <c r="I955">
+        <v>59</v>
+      </c>
+      <c r="J955" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K955">
+        <v>53.06</v>
+      </c>
+      <c r="L955">
+        <v>49.27</v>
+      </c>
+      <c r="M955">
+        <v>16.27</v>
+      </c>
+      <c r="N955" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="956" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A956" t="s">
+        <v>11</v>
+      </c>
+      <c r="B956" t="s">
+        <v>12</v>
+      </c>
+      <c r="C956" t="s">
+        <v>13</v>
+      </c>
+      <c r="D956" t="s">
+        <v>16</v>
+      </c>
+      <c r="E956" t="s">
+        <v>15</v>
+      </c>
+      <c r="F956" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G956" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H956">
+        <v>3</v>
+      </c>
+      <c r="I956">
+        <v>59</v>
+      </c>
+      <c r="J956" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K956">
+        <v>58.4</v>
+      </c>
+      <c r="L956">
+        <v>43.64</v>
+      </c>
+      <c r="M956">
+        <v>16.440000000000001</v>
+      </c>
+      <c r="N956" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="957" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A957" t="s">
+        <v>11</v>
+      </c>
+      <c r="B957" t="s">
+        <v>12</v>
+      </c>
+      <c r="C957" t="s">
+        <v>13</v>
+      </c>
+      <c r="D957" t="s">
+        <v>16</v>
+      </c>
+      <c r="E957" t="s">
+        <v>15</v>
+      </c>
+      <c r="F957" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G957" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H957">
+        <v>3</v>
+      </c>
+      <c r="I957">
+        <v>59</v>
+      </c>
+      <c r="J957" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K957">
+        <v>51.07</v>
+      </c>
+      <c r="L957">
+        <v>30.2</v>
+      </c>
+      <c r="M957">
+        <v>13.47</v>
+      </c>
+      <c r="N957" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="958" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A958" t="s">
+        <v>11</v>
+      </c>
+      <c r="B958" t="s">
+        <v>12</v>
+      </c>
+      <c r="C958" t="s">
+        <v>13</v>
+      </c>
+      <c r="D958" t="s">
+        <v>16</v>
+      </c>
+      <c r="E958" t="s">
+        <v>15</v>
+      </c>
+      <c r="F958" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G958" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H958">
+        <v>3</v>
+      </c>
+      <c r="I958">
+        <v>59</v>
+      </c>
+      <c r="J958" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K958">
+        <v>57.93</v>
+      </c>
+      <c r="L958">
+        <v>50.72</v>
+      </c>
+      <c r="M958">
+        <v>22.09</v>
+      </c>
+      <c r="N958" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="959" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A959" t="s">
+        <v>11</v>
+      </c>
+      <c r="B959" t="s">
+        <v>12</v>
+      </c>
+      <c r="C959" t="s">
+        <v>13</v>
+      </c>
+      <c r="D959" t="s">
+        <v>16</v>
+      </c>
+      <c r="E959" t="s">
+        <v>15</v>
+      </c>
+      <c r="F959" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G959" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H959">
+        <v>3</v>
+      </c>
+      <c r="I959">
+        <v>59</v>
+      </c>
+      <c r="J959" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K959">
+        <v>46.58</v>
+      </c>
+      <c r="L959">
+        <v>42.19</v>
+      </c>
+      <c r="M959">
+        <v>20.55</v>
+      </c>
+      <c r="N959" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="960" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A960" t="s">
+        <v>11</v>
+      </c>
+      <c r="B960" t="s">
+        <v>12</v>
+      </c>
+      <c r="C960" t="s">
+        <v>13</v>
+      </c>
+      <c r="D960" t="s">
+        <v>16</v>
+      </c>
+      <c r="E960" t="s">
+        <v>15</v>
+      </c>
+      <c r="F960" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G960" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H960">
+        <v>3</v>
+      </c>
+      <c r="I960">
+        <v>59</v>
+      </c>
+      <c r="J960" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K960">
+        <v>45.21</v>
+      </c>
+      <c r="L960">
+        <v>35.86</v>
+      </c>
+      <c r="M960">
+        <v>16.23</v>
+      </c>
+      <c r="N960" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="961" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A961" t="s">
+        <v>11</v>
+      </c>
+      <c r="B961" t="s">
+        <v>12</v>
+      </c>
+      <c r="C961" t="s">
+        <v>13</v>
+      </c>
+      <c r="D961" t="s">
+        <v>16</v>
+      </c>
+      <c r="E961" t="s">
+        <v>15</v>
+      </c>
+      <c r="F961" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G961" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H961">
+        <v>3</v>
+      </c>
+      <c r="I961">
+        <v>59</v>
+      </c>
+      <c r="J961" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K961">
+        <v>59.91</v>
+      </c>
+      <c r="L961">
+        <v>49.82</v>
+      </c>
+      <c r="M961">
+        <v>21.42</v>
+      </c>
+      <c r="N961" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="962" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A962" t="s">
+        <v>11</v>
+      </c>
+      <c r="B962" t="s">
+        <v>12</v>
+      </c>
+      <c r="C962" t="s">
+        <v>13</v>
+      </c>
+      <c r="D962" t="s">
+        <v>14</v>
+      </c>
+      <c r="E962" t="s">
+        <v>15</v>
+      </c>
+      <c r="F962" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G962" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H962">
+        <v>8</v>
+      </c>
+      <c r="I962">
+        <v>62</v>
+      </c>
+      <c r="J962" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K962">
+        <v>72.010000000000005</v>
+      </c>
+      <c r="L962">
+        <v>52.12</v>
+      </c>
+      <c r="M962">
+        <v>18.04</v>
+      </c>
+      <c r="N962" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="963" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A963" t="s">
+        <v>11</v>
+      </c>
+      <c r="B963" t="s">
+        <v>12</v>
+      </c>
+      <c r="C963" t="s">
+        <v>13</v>
+      </c>
+      <c r="D963" t="s">
+        <v>14</v>
+      </c>
+      <c r="E963" t="s">
+        <v>15</v>
+      </c>
+      <c r="F963" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G963" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H963">
+        <v>8</v>
+      </c>
+      <c r="I963">
+        <v>62</v>
+      </c>
+      <c r="J963" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K963">
+        <v>47.83</v>
+      </c>
+      <c r="L963">
+        <v>32.79</v>
+      </c>
+      <c r="M963">
+        <v>16.45</v>
+      </c>
+      <c r="N963" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="964" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A964" t="s">
+        <v>11</v>
+      </c>
+      <c r="B964" t="s">
+        <v>12</v>
+      </c>
+      <c r="C964" t="s">
+        <v>13</v>
+      </c>
+      <c r="D964" t="s">
+        <v>14</v>
+      </c>
+      <c r="E964" t="s">
+        <v>15</v>
+      </c>
+      <c r="F964" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G964" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H964">
+        <v>8</v>
+      </c>
+      <c r="I964">
+        <v>62</v>
+      </c>
+      <c r="J964" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K964">
+        <v>53.15</v>
+      </c>
+      <c r="L964">
+        <v>37.15</v>
+      </c>
+      <c r="M964">
+        <v>18.760000000000002</v>
+      </c>
+      <c r="N964" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="965" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A965" t="s">
+        <v>11</v>
+      </c>
+      <c r="B965" t="s">
+        <v>12</v>
+      </c>
+      <c r="C965" t="s">
+        <v>13</v>
+      </c>
+      <c r="D965" t="s">
+        <v>14</v>
+      </c>
+      <c r="E965" t="s">
+        <v>15</v>
+      </c>
+      <c r="F965" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G965" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H965">
+        <v>8</v>
+      </c>
+      <c r="I965">
+        <v>62</v>
+      </c>
+      <c r="J965" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K965">
+        <v>50.06</v>
+      </c>
+      <c r="L965">
+        <v>28.4</v>
+      </c>
+      <c r="M965">
+        <v>17.64</v>
+      </c>
+      <c r="N965" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="966" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A966" t="s">
+        <v>11</v>
+      </c>
+      <c r="B966" t="s">
+        <v>12</v>
+      </c>
+      <c r="C966" t="s">
+        <v>13</v>
+      </c>
+      <c r="D966" t="s">
+        <v>14</v>
+      </c>
+      <c r="E966" t="s">
+        <v>15</v>
+      </c>
+      <c r="F966" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G966" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H966">
+        <v>8</v>
+      </c>
+      <c r="I966">
+        <v>62</v>
+      </c>
+      <c r="J966" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K966">
+        <v>43.8</v>
+      </c>
+      <c r="L966">
+        <v>43.03</v>
+      </c>
+      <c r="M966">
+        <v>18.36</v>
+      </c>
+      <c r="N966" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="967" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A967" t="s">
+        <v>11</v>
+      </c>
+      <c r="B967" t="s">
+        <v>12</v>
+      </c>
+      <c r="C967" t="s">
+        <v>13</v>
+      </c>
+      <c r="D967" t="s">
+        <v>14</v>
+      </c>
+      <c r="E967" t="s">
+        <v>15</v>
+      </c>
+      <c r="F967" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G967" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H967">
+        <v>8</v>
+      </c>
+      <c r="I967">
+        <v>62</v>
+      </c>
+      <c r="J967" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K967">
+        <v>73.53</v>
+      </c>
+      <c r="L967">
+        <v>41.2</v>
+      </c>
+      <c r="M967">
+        <v>21.85</v>
+      </c>
+      <c r="N967" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="968" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A968" t="s">
+        <v>11</v>
+      </c>
+      <c r="B968" t="s">
+        <v>12</v>
+      </c>
+      <c r="C968" t="s">
+        <v>13</v>
+      </c>
+      <c r="D968" t="s">
+        <v>14</v>
+      </c>
+      <c r="E968" t="s">
+        <v>15</v>
+      </c>
+      <c r="F968" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G968" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H968">
+        <v>8</v>
+      </c>
+      <c r="I968">
+        <v>62</v>
+      </c>
+      <c r="J968" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K968">
+        <v>55.78</v>
+      </c>
+      <c r="L968">
+        <v>42.87</v>
+      </c>
+      <c r="M968">
+        <v>20.86</v>
+      </c>
+      <c r="N968" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="969" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A969" t="s">
+        <v>11</v>
+      </c>
+      <c r="B969" t="s">
+        <v>12</v>
+      </c>
+      <c r="C969" t="s">
+        <v>13</v>
+      </c>
+      <c r="D969" t="s">
+        <v>14</v>
+      </c>
+      <c r="E969" t="s">
+        <v>15</v>
+      </c>
+      <c r="F969" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G969" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H969">
+        <v>8</v>
+      </c>
+      <c r="I969">
+        <v>62</v>
+      </c>
+      <c r="J969" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K969">
+        <v>69.53</v>
+      </c>
+      <c r="L969">
+        <v>48.56</v>
+      </c>
+      <c r="M969">
+        <v>25.59</v>
+      </c>
+      <c r="N969" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="970" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A970" t="s">
+        <v>11</v>
+      </c>
+      <c r="B970" t="s">
+        <v>12</v>
+      </c>
+      <c r="C970" t="s">
+        <v>13</v>
+      </c>
+      <c r="D970" t="s">
+        <v>14</v>
+      </c>
+      <c r="E970" t="s">
+        <v>15</v>
+      </c>
+      <c r="F970" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G970" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H970">
+        <v>8</v>
+      </c>
+      <c r="I970">
+        <v>62</v>
+      </c>
+      <c r="J970" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K970">
+        <v>59.18</v>
+      </c>
+      <c r="L970">
+        <v>34.270000000000003</v>
+      </c>
+      <c r="M970">
+        <v>14.62</v>
+      </c>
+      <c r="N970" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="971" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A971" t="s">
+        <v>11</v>
+      </c>
+      <c r="B971" t="s">
+        <v>12</v>
+      </c>
+      <c r="C971" t="s">
+        <v>13</v>
+      </c>
+      <c r="D971" t="s">
+        <v>14</v>
+      </c>
+      <c r="E971" t="s">
+        <v>15</v>
+      </c>
+      <c r="F971" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G971" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H971">
+        <v>8</v>
+      </c>
+      <c r="I971">
+        <v>62</v>
+      </c>
+      <c r="J971" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K971">
+        <v>59.35</v>
+      </c>
+      <c r="L971">
+        <v>41.34</v>
+      </c>
+      <c r="M971">
+        <v>17.940000000000001</v>
+      </c>
+      <c r="N971" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="972" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A972" t="s">
+        <v>11</v>
+      </c>
+      <c r="B972" t="s">
+        <v>12</v>
+      </c>
+      <c r="C972" t="s">
+        <v>13</v>
+      </c>
+      <c r="D972" t="s">
+        <v>16</v>
+      </c>
+      <c r="E972" t="s">
+        <v>15</v>
+      </c>
+      <c r="F972" s="1">
+        <v>45862</v>
+      </c>
+      <c r="G972" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H972">
+        <v>5</v>
+      </c>
+      <c r="I972">
+        <v>73</v>
+      </c>
+      <c r="K972">
+        <v>83.44</v>
+      </c>
+      <c r="L972">
+        <v>50.74</v>
+      </c>
+    </row>
+    <row r="973" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K973">
+        <v>31.18</v>
+      </c>
+      <c r="L973">
+        <v>36.979999999999997</v>
+      </c>
+    </row>
+    <row r="974" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K974">
+        <v>61.53</v>
+      </c>
+      <c r="L974">
+        <v>46.93</v>
+      </c>
+    </row>
+    <row r="975" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K975">
+        <v>46.26</v>
+      </c>
+      <c r="L975">
+        <v>39.81</v>
+      </c>
+    </row>
+    <row r="976" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K976">
+        <v>65.400000000000006</v>
+      </c>
+    </row>
+    <row r="977" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K977">
+        <v>89.17</v>
+      </c>
+    </row>
+    <row r="978" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K978">
+        <v>76.040000000000006</v>
+      </c>
+    </row>
+    <row r="979" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K979">
+        <v>71.06</v>
+      </c>
+    </row>
+    <row r="980" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K980">
+        <v>49.2</v>
+      </c>
+    </row>
+    <row r="981" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K981">
+        <v>50.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>